<commit_message>
Corrected few things and started indicator reporting
</commit_message>
<xml_diff>
--- a/report/ECMENIndicators.xlsx
+++ b/report/ECMENIndicators.xlsx
@@ -1,61 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wfp-my.sharepoint.com/personal/eltone_mabodo_wfp_org/Documents/Documents/Work 2023 -Eltone/General M&amp;E/GASFP Project/gasfp-outcome-survey/report/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_C2CE303C9899E5F86D68441C1D0A53129275BF39" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74E61387-B447-498A-80C6-56C202C2F52B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">ECMENStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disagregation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Able to meet essential needs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unable to meet essential needs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethnic Majority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethnic Minority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foreigners</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+  <si>
+    <t>ECMENStatus</t>
+  </si>
+  <si>
+    <t>Disagregation</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Able to meet essential needs</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Unable to meet essential needs</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Ethnic Majority</t>
+  </si>
+  <si>
+    <t>Ethnic Minority</t>
+  </si>
+  <si>
+    <t>Baseline Members</t>
+  </si>
+  <si>
+    <t>New Members</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,6 +101,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -372,14 +391,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,176 +417,204 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>171</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>48.86</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>179</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>51.14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>58</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>44.96</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>71</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>55.04</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>113</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>51.13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>108</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>48.87</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>100</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>63.29</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>58</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>36.71</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>68</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>36.56</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>118</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>63.44</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="C12">
+        <v>134</v>
+      </c>
+      <c r="D12">
+        <v>60.91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" t="n">
-        <v>50</v>
+      <c r="C13">
+        <v>86</v>
+      </c>
+      <c r="D13">
+        <v>39.090000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>28.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>91</v>
+      </c>
+      <c r="D15">
+        <v>71.650000000000006</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>